<commit_message>
Signed-off-by: Andrei Driuk <andredryuk@yandex.com>
</commit_message>
<xml_diff>
--- a/Результаты.xlsx
+++ b/Результаты.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intro_in_mod_prog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C115B661-A3B4-4713-B347-7F8476B513C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E49107-939E-42BC-BE6E-78E3C64D1380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E6D91174-602C-473A-A8FB-74C0D0C45DD2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Группа</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Олег Башкирцев</t>
+  </si>
+  <si>
+    <t>Олег Шестопалов</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35E24D9-2ED9-481A-9E29-09A01E5F7056}">
-  <dimension ref="E7:K21"/>
+  <dimension ref="E7:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F7" sqref="F7:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,6 +606,12 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>